<commit_message>
Ipmlicit, Explicit wait java files uploaded.
</commit_message>
<xml_diff>
--- a/Volaris/inputFiles/testData.xlsx
+++ b/Volaris/inputFiles/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14190" windowHeight="5985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13845" windowHeight="5985"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,44 +13,26 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N17"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>user1</t>
-  </si>
-  <si>
-    <t>pass1</t>
   </si>
   <si>
     <t>user2</t>
   </si>
   <si>
-    <t>pass2</t>
-  </si>
-  <si>
     <t>user3</t>
-  </si>
-  <si>
-    <t>pass3</t>
   </si>
   <si>
     <t>amar</t>
   </si>
   <si>
     <t>nath</t>
-  </si>
-  <si>
-    <t>Mobile1</t>
-  </si>
-  <si>
-    <t>March/03/2017</t>
-  </si>
-  <si>
-    <t>FALSE/TRUE</t>
   </si>
 </sst>
 </file>
@@ -397,7 +379,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,11 +392,8 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
+      <c r="B1">
+        <v>12</v>
       </c>
       <c r="D1" t="b">
         <v>1</v>
@@ -422,13 +401,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>23</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -436,50 +412,22 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>34</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>123456</v>
-      </c>
-      <c r="B4">
-        <v>45678</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-    </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>42950</v>
-      </c>
-      <c r="B5" s="1">
-        <v>42802</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>42797</v>
-      </c>
+      <c r="A6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -498,10 +446,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>